<commit_message>
Try / Except loop added to user inputs to avoid error messages
</commit_message>
<xml_diff>
--- a/SAC_within.xlsx
+++ b/SAC_within.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,16 +467,16 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>21</v>
+        <v>217</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>000106</t>
+          <t>001058</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>St. Gobnet's Wood SAC</t>
+          <t>Great Island Channel SAC</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -485,231 +485,14 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>43.8515821375</v>
+        <v>1437.549977</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>3.00999999046</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.npws.ie/protected-sites/sac/000106</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>000108</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>The Gearagh SAC</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>co</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>554.173594</v>
-      </c>
-      <c r="F3" t="n">
-        <v>3.00999999046</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>https://www.npws.ie/protected-sites/sac/000108</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>000365</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Killarney National Park, Macgillycuddy's Reeks And Caragh River Catchment SAC</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>co</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>1463.59315438</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>https://www.npws.ie/protected-sites/sac/000365</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>000365</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Killarney National Park, Macgillycuddy's Reeks And Caragh River Catchment SAC</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>ke</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>74981.3962511</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1.19000005722</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>https://www.npws.ie/protected-sites/sac/000365</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>285</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>001890</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Mullaghanish Bog SAC</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>co</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>60.19001</v>
-      </c>
-      <c r="F6" t="n">
-        <v>3</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>https://www.npws.ie/protected-sites/sac/001890</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>362</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>002170</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Blackwater River (Cork/Waterford) SAC</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>co</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>6248.56605951</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1.14999997616</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>https://www.npws.ie/protected-sites/sac/002170</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>363</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>002170</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Blackwater River (Cork/Waterford) SAC</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>ke</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>212.464051565</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1.03999996185</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>https://www.npws.ie/protected-sites/sac/002170</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>367</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>002171</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Bandon River SAC</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>co</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>317.573318484</v>
-      </c>
-      <c r="F9" t="n">
-        <v>3.00999999046</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>https://www.npws.ie/protected-sites/sac/002171</t>
+          <t>https://www.npws.ie/protected-sites/sac/001058</t>
         </is>
       </c>
     </row>

</xml_diff>